<commit_message>
commit the df_toyota after correctly null values at column security
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_toyota_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_toyota_updated.xlsx
@@ -472,7 +472,11 @@
           <t>4 Runner</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -491,7 +495,11 @@
           <t>Avalon</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -510,7 +518,11 @@
           <t>Camry</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -529,7 +541,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -548,7 +564,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -567,7 +587,11 @@
           <t>Landcruiser</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -586,7 +610,11 @@
           <t>RAV 4</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -605,7 +633,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -624,7 +656,11 @@
           <t>4 Runner</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -643,7 +679,11 @@
           <t>Avalon</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -662,7 +702,11 @@
           <t>Camry</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -681,7 +725,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -700,7 +748,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -719,7 +771,11 @@
           <t>Landcruiser</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -738,7 +794,11 @@
           <t>RAV 4</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -757,7 +817,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -776,7 +840,11 @@
           <t>4 Runner</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -795,7 +863,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -814,7 +886,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -833,7 +909,11 @@
           <t>RAV 4</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -852,7 +932,11 @@
           <t>Sienna</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -871,7 +955,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -959,7 +1047,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -978,7 +1070,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -997,7 +1093,11 @@
           <t>RAV 4</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1016,7 +1116,11 @@
           <t>Sienna</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1035,7 +1139,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1169,7 +1277,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1188,7 +1300,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1207,7 +1323,11 @@
           <t>Echo</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1226,7 +1346,11 @@
           <t>RAV 4</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1245,7 +1369,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1264,7 +1392,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1444,7 +1576,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1463,7 +1599,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1482,7 +1622,11 @@
           <t>Echo</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1501,7 +1645,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1520,7 +1668,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1792,7 +1944,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1811,7 +1967,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1830,7 +1990,11 @@
           <t>Echo</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1849,7 +2013,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1868,7 +2036,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2140,7 +2312,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2159,7 +2335,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2178,7 +2358,11 @@
           <t>Echo</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2197,7 +2381,11 @@
           <t>Matrix</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2216,7 +2404,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2235,7 +2427,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2507,7 +2703,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2526,7 +2726,11 @@
           <t>Corolla</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2545,7 +2749,11 @@
           <t>Echo</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2564,7 +2772,11 @@
           <t>Matrix</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr"/>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -2583,7 +2795,11 @@
           <t>Tacoma</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -2602,7 +2818,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr"/>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -2874,7 +3094,11 @@
           <t>Celica</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -2893,7 +3117,11 @@
           <t>Echo</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -2912,7 +3140,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -3276,7 +3508,11 @@
           <t>FJ Cruiser</t>
         </is>
       </c>
-      <c r="E134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -3295,7 +3531,11 @@
           <t>Tundra</t>
         </is>
       </c>
-      <c r="E135" t="inlineStr"/>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -3636,7 +3876,11 @@
           <t>FJ Cruiser</t>
         </is>
       </c>
-      <c r="E150" t="inlineStr"/>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -3655,7 +3899,11 @@
           <t>Yaris</t>
         </is>
       </c>
-      <c r="E151" t="inlineStr"/>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">

</xml_diff>